<commit_message>
udalost je radek s hodnotou v kteremkoliv sloupci
</commit_message>
<xml_diff>
--- a/test/test.xlsx
+++ b/test/test.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26215"/>
   <workbookPr showInkAnnotation="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mira/Desktop/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="24240" windowHeight="13740" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="34540" windowHeight="17980" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="39">
   <si>
     <t>1.</t>
   </si>
@@ -34,12 +39,6 @@
   </si>
   <si>
     <t>divadlo Druhý Pád</t>
-  </si>
-  <si>
-    <t>4.</t>
-  </si>
-  <si>
-    <t>19.00</t>
   </si>
   <si>
     <t>Curanderos</t>
@@ -529,7 +528,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -542,61 +541,61 @@
   </sheetPr>
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="B5" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.625" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" customWidth="1"/>
     <col min="4" max="4" width="34.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="60" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="H1" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D4" t="s">
         <v>2</v>
       </c>
@@ -604,109 +603,100 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E5" t="s">
         <v>5</v>
       </c>
-      <c r="D5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
         <v>10</v>
       </c>
-      <c r="C6" t="s">
+      <c r="E6" t="s">
         <v>11</v>
-      </c>
-      <c r="D6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" t="s">
         <v>21</v>
       </c>
-      <c r="D8" t="s">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
         <v>22</v>
       </c>
-      <c r="E8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>24</v>
-      </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C11" t="s">
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" t="s">
         <v>18</v>
       </c>
-      <c r="C12" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" t="s">
-        <v>20</v>
-      </c>
       <c r="E12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H13" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>0</v>
       </c>
@@ -720,85 +710,58 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D15" t="s">
         <v>4</v>
       </c>
-      <c r="C15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" t="s">
-        <v>6</v>
-      </c>
-      <c r="E15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" t="s">
         <v>10</v>
       </c>
-      <c r="C16" t="s">
+      <c r="E16" t="s">
         <v>11</v>
       </c>
-      <c r="D16" t="s">
-        <v>12</v>
-      </c>
-      <c r="E16" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18" t="s">
         <v>21</v>
       </c>
-      <c r="D18" t="s">
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
         <v>22</v>
-      </c>
-      <c r="E18" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>24</v>
-      </c>
-      <c r="C19" t="s">
-        <v>8</v>
-      </c>
-      <c r="D19" t="s">
-        <v>14</v>
-      </c>
-      <c r="E19" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C21" t="s">
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E21" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>18</v>
-      </c>
-      <c r="C22" t="s">
-        <v>19</v>
-      </c>
-      <c r="D22" t="s">
-        <v>20</v>
-      </c>
-      <c r="E22" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>